<commit_message>
2021-05-04 14:33:20 - Update
</commit_message>
<xml_diff>
--- a/swap.xlsx
+++ b/swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4496,6 +4496,206 @@
         <v>42793</v>
       </c>
     </row>
+    <row r="83">
+      <c r="A83" s="2">
+        <v>44314</v>
+      </c>
+      <c r="B83">
+        <v>485</v>
+      </c>
+      <c r="C83">
+        <v>3566</v>
+      </c>
+      <c r="D83">
+        <v>1300</v>
+      </c>
+      <c r="E83">
+        <v>5601</v>
+      </c>
+      <c r="F83">
+        <v>131</v>
+      </c>
+      <c r="G83">
+        <v>1666</v>
+      </c>
+      <c r="H83">
+        <v>1000</v>
+      </c>
+      <c r="I83">
+        <v>28500</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <v>3638</v>
+      </c>
+      <c r="N83">
+        <v>144</v>
+      </c>
+      <c r="O83">
+        <v>1081</v>
+      </c>
+      <c r="P83">
+        <v>42971</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2">
+        <v>44315</v>
+      </c>
+      <c r="B84">
+        <v>1270</v>
+      </c>
+      <c r="C84">
+        <v>3616</v>
+      </c>
+      <c r="D84">
+        <v>800</v>
+      </c>
+      <c r="E84">
+        <v>5651</v>
+      </c>
+      <c r="F84">
+        <v>188</v>
+      </c>
+      <c r="G84">
+        <v>1835</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>28500</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>3638</v>
+      </c>
+      <c r="N84">
+        <v>597</v>
+      </c>
+      <c r="O84">
+        <v>1138</v>
+      </c>
+      <c r="P84">
+        <v>43241</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2">
+        <v>44316</v>
+      </c>
+      <c r="B85">
+        <v>40</v>
+      </c>
+      <c r="C85">
+        <v>3531</v>
+      </c>
+      <c r="D85">
+        <v>850</v>
+      </c>
+      <c r="E85">
+        <v>5601</v>
+      </c>
+      <c r="F85">
+        <v>725</v>
+      </c>
+      <c r="G85">
+        <v>1946</v>
+      </c>
+      <c r="H85">
+        <v>1000</v>
+      </c>
+      <c r="I85">
+        <v>28500</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>3638</v>
+      </c>
+      <c r="N85">
+        <v>11</v>
+      </c>
+      <c r="O85">
+        <v>1126</v>
+      </c>
+      <c r="P85">
+        <v>43217</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2">
+        <v>44319</v>
+      </c>
+      <c r="B86">
+        <v>433</v>
+      </c>
+      <c r="C86">
+        <v>3333</v>
+      </c>
+      <c r="D86">
+        <v>740</v>
+      </c>
+      <c r="E86">
+        <v>5751</v>
+      </c>
+      <c r="F86">
+        <v>683</v>
+      </c>
+      <c r="G86">
+        <v>1929</v>
+      </c>
+      <c r="H86">
+        <v>1000</v>
+      </c>
+      <c r="I86">
+        <v>28500</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86">
+        <v>3638</v>
+      </c>
+      <c r="N86">
+        <v>182</v>
+      </c>
+      <c r="O86">
+        <v>1124</v>
+      </c>
+      <c r="P86">
+        <v>43151</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2021-05-06 15:13:41 - Update
</commit_message>
<xml_diff>
--- a/swap.xlsx
+++ b/swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4696,6 +4696,106 @@
         <v>43151</v>
       </c>
     </row>
+    <row r="87">
+      <c r="A87" s="2">
+        <v>44320</v>
+      </c>
+      <c r="B87">
+        <v>710</v>
+      </c>
+      <c r="C87">
+        <v>2938</v>
+      </c>
+      <c r="D87">
+        <v>550</v>
+      </c>
+      <c r="E87">
+        <v>5601</v>
+      </c>
+      <c r="F87">
+        <v>201</v>
+      </c>
+      <c r="G87">
+        <v>1927</v>
+      </c>
+      <c r="H87">
+        <v>1000</v>
+      </c>
+      <c r="I87">
+        <v>28500</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+      <c r="K87">
+        <v>0</v>
+      </c>
+      <c r="L87">
+        <v>0</v>
+      </c>
+      <c r="M87">
+        <v>3638</v>
+      </c>
+      <c r="N87">
+        <v>265</v>
+      </c>
+      <c r="O87">
+        <v>1200</v>
+      </c>
+      <c r="P87">
+        <v>42605</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2">
+        <v>44321</v>
+      </c>
+      <c r="B88">
+        <v>250</v>
+      </c>
+      <c r="C88">
+        <v>2703</v>
+      </c>
+      <c r="D88">
+        <v>870</v>
+      </c>
+      <c r="E88">
+        <v>5525</v>
+      </c>
+      <c r="F88">
+        <v>131</v>
+      </c>
+      <c r="G88">
+        <v>1928</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>28500</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88">
+        <v>0</v>
+      </c>
+      <c r="L88">
+        <v>0</v>
+      </c>
+      <c r="M88">
+        <v>3638</v>
+      </c>
+      <c r="N88">
+        <v>158</v>
+      </c>
+      <c r="O88">
+        <v>1213</v>
+      </c>
+      <c r="P88">
+        <v>42294</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2021-05-18 15:30:18 - Update
</commit_message>
<xml_diff>
--- a/swap.xlsx
+++ b/swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P88"/>
+  <dimension ref="A1:P94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -4796,6 +4796,306 @@
         <v>42294</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89" s="2">
+        <v>44322</v>
+      </c>
+      <c r="B89">
+        <v>1045</v>
+      </c>
+      <c r="C89">
+        <v>2478</v>
+      </c>
+      <c r="D89">
+        <v>615</v>
+      </c>
+      <c r="E89">
+        <v>5425</v>
+      </c>
+      <c r="F89">
+        <v>189</v>
+      </c>
+      <c r="G89">
+        <v>1929</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <v>28500</v>
+      </c>
+      <c r="J89">
+        <v>0</v>
+      </c>
+      <c r="K89">
+        <v>0</v>
+      </c>
+      <c r="L89">
+        <v>0</v>
+      </c>
+      <c r="M89">
+        <v>3638</v>
+      </c>
+      <c r="N89">
+        <v>310</v>
+      </c>
+      <c r="O89">
+        <v>925</v>
+      </c>
+      <c r="P89">
+        <v>41971</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2">
+        <v>44323</v>
+      </c>
+      <c r="B90">
+        <v>450</v>
+      </c>
+      <c r="C90">
+        <v>2888</v>
+      </c>
+      <c r="D90">
+        <v>850</v>
+      </c>
+      <c r="E90">
+        <v>5325</v>
+      </c>
+      <c r="F90">
+        <v>724</v>
+      </c>
+      <c r="G90">
+        <v>1928</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90">
+        <v>28500</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+      <c r="K90">
+        <v>0</v>
+      </c>
+      <c r="L90">
+        <v>0</v>
+      </c>
+      <c r="M90">
+        <v>3638</v>
+      </c>
+      <c r="N90">
+        <v>11</v>
+      </c>
+      <c r="O90">
+        <v>925</v>
+      </c>
+      <c r="P90">
+        <v>42279</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2">
+        <v>44326</v>
+      </c>
+      <c r="B91">
+        <v>671</v>
+      </c>
+      <c r="C91">
+        <v>3126</v>
+      </c>
+      <c r="D91">
+        <v>850</v>
+      </c>
+      <c r="E91">
+        <v>5275</v>
+      </c>
+      <c r="F91">
+        <v>686</v>
+      </c>
+      <c r="G91">
+        <v>1931</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+      <c r="I91">
+        <v>28500</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+      <c r="K91">
+        <v>0</v>
+      </c>
+      <c r="L91">
+        <v>0</v>
+      </c>
+      <c r="M91">
+        <v>3638</v>
+      </c>
+      <c r="N91">
+        <v>135</v>
+      </c>
+      <c r="O91">
+        <v>878</v>
+      </c>
+      <c r="P91">
+        <v>42470</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2">
+        <v>44327</v>
+      </c>
+      <c r="B92">
+        <v>530</v>
+      </c>
+      <c r="C92">
+        <v>2946</v>
+      </c>
+      <c r="D92">
+        <v>800</v>
+      </c>
+      <c r="E92">
+        <v>5275</v>
+      </c>
+      <c r="F92">
+        <v>208</v>
+      </c>
+      <c r="G92">
+        <v>1938</v>
+      </c>
+      <c r="H92">
+        <v>1000</v>
+      </c>
+      <c r="I92">
+        <v>28500</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+      <c r="K92">
+        <v>0</v>
+      </c>
+      <c r="L92">
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <v>3638</v>
+      </c>
+      <c r="N92">
+        <v>224</v>
+      </c>
+      <c r="O92">
+        <v>837</v>
+      </c>
+      <c r="P92">
+        <v>42298</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2">
+        <v>44328</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+      <c r="C93">
+        <v>2946</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>5275</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>1938</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93">
+        <v>28500</v>
+      </c>
+      <c r="J93">
+        <v>0</v>
+      </c>
+      <c r="K93">
+        <v>0</v>
+      </c>
+      <c r="L93">
+        <v>0</v>
+      </c>
+      <c r="M93">
+        <v>3638</v>
+      </c>
+      <c r="N93">
+        <v>0</v>
+      </c>
+      <c r="O93">
+        <v>837</v>
+      </c>
+      <c r="P93">
+        <v>42298</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2">
+        <v>44333</v>
+      </c>
+      <c r="B94">
+        <v>741</v>
+      </c>
+      <c r="C94">
+        <v>3016</v>
+      </c>
+      <c r="D94">
+        <v>1172</v>
+      </c>
+      <c r="E94">
+        <v>5677</v>
+      </c>
+      <c r="F94">
+        <v>781</v>
+      </c>
+      <c r="G94">
+        <v>2034</v>
+      </c>
+      <c r="H94">
+        <v>1000</v>
+      </c>
+      <c r="I94">
+        <v>28500</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+      <c r="K94">
+        <v>0</v>
+      </c>
+      <c r="L94">
+        <v>1235</v>
+      </c>
+      <c r="M94">
+        <v>3674</v>
+      </c>
+      <c r="N94">
+        <v>436</v>
+      </c>
+      <c r="O94">
+        <v>1138</v>
+      </c>
+      <c r="P94">
+        <v>42901</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2021-05-20 13:41:03 - Update
</commit_message>
<xml_diff>
--- a/swap.xlsx
+++ b/swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P94"/>
+  <dimension ref="A1:P95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5096,6 +5096,56 @@
         <v>42901</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" s="2">
+        <v>44334</v>
+      </c>
+      <c r="B95">
+        <v>515</v>
+      </c>
+      <c r="C95">
+        <v>3001</v>
+      </c>
+      <c r="D95">
+        <v>900</v>
+      </c>
+      <c r="E95">
+        <v>6077</v>
+      </c>
+      <c r="F95">
+        <v>253</v>
+      </c>
+      <c r="G95">
+        <v>2079</v>
+      </c>
+      <c r="H95">
+        <v>1000</v>
+      </c>
+      <c r="I95">
+        <v>28500</v>
+      </c>
+      <c r="J95">
+        <v>0</v>
+      </c>
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <v>3674</v>
+      </c>
+      <c r="N95">
+        <v>184</v>
+      </c>
+      <c r="O95">
+        <v>1099</v>
+      </c>
+      <c r="P95">
+        <v>43330</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2021-05-23 17:18:13 - Update
</commit_message>
<xml_diff>
--- a/swap.xlsx
+++ b/swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P95"/>
+  <dimension ref="A1:P97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5146,6 +5146,106 @@
         <v>43330</v>
       </c>
     </row>
+    <row r="96">
+      <c r="A96" s="2">
+        <v>44336</v>
+      </c>
+      <c r="B96">
+        <v>905</v>
+      </c>
+      <c r="C96">
+        <v>2611</v>
+      </c>
+      <c r="D96">
+        <v>650</v>
+      </c>
+      <c r="E96">
+        <v>5977</v>
+      </c>
+      <c r="F96">
+        <v>450</v>
+      </c>
+      <c r="G96">
+        <v>2209</v>
+      </c>
+      <c r="H96">
+        <v>1000</v>
+      </c>
+      <c r="I96">
+        <v>28500</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>3674</v>
+      </c>
+      <c r="N96">
+        <v>509</v>
+      </c>
+      <c r="O96">
+        <v>1140</v>
+      </c>
+      <c r="P96">
+        <v>42970</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2">
+        <v>44337</v>
+      </c>
+      <c r="B97">
+        <v>350</v>
+      </c>
+      <c r="C97">
+        <v>2511</v>
+      </c>
+      <c r="D97">
+        <v>755</v>
+      </c>
+      <c r="E97">
+        <v>5827</v>
+      </c>
+      <c r="F97">
+        <v>517</v>
+      </c>
+      <c r="G97">
+        <v>2002</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+      <c r="I97">
+        <v>28500</v>
+      </c>
+      <c r="J97">
+        <v>0</v>
+      </c>
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>3674</v>
+      </c>
+      <c r="N97">
+        <v>24</v>
+      </c>
+      <c r="O97">
+        <v>1153</v>
+      </c>
+      <c r="P97">
+        <v>42514</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2021-06-04 02:35:41 - Update
</commit_message>
<xml_diff>
--- a/swap.xlsx
+++ b/swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P97"/>
+  <dimension ref="A1:P106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5246,6 +5246,456 @@
         <v>42514</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" s="2">
+        <v>44340</v>
+      </c>
+      <c r="B98">
+        <v>631</v>
+      </c>
+      <c r="C98">
+        <v>2401</v>
+      </c>
+      <c r="D98">
+        <v>1050</v>
+      </c>
+      <c r="E98">
+        <v>6177</v>
+      </c>
+      <c r="F98">
+        <v>967</v>
+      </c>
+      <c r="G98">
+        <v>2188</v>
+      </c>
+      <c r="H98">
+        <v>1000</v>
+      </c>
+      <c r="I98">
+        <v>28500</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>3674</v>
+      </c>
+      <c r="N98">
+        <v>356</v>
+      </c>
+      <c r="O98">
+        <v>1073</v>
+      </c>
+      <c r="P98">
+        <v>42939</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2">
+        <v>44341</v>
+      </c>
+      <c r="B99">
+        <v>415</v>
+      </c>
+      <c r="C99">
+        <v>2301</v>
+      </c>
+      <c r="D99">
+        <v>672</v>
+      </c>
+      <c r="E99">
+        <v>5927</v>
+      </c>
+      <c r="F99">
+        <v>218</v>
+      </c>
+      <c r="G99">
+        <v>2153</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+      <c r="I99">
+        <v>28500</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>3674</v>
+      </c>
+      <c r="N99">
+        <v>226</v>
+      </c>
+      <c r="O99">
+        <v>1115</v>
+      </c>
+      <c r="P99">
+        <v>42554</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2">
+        <v>44342</v>
+      </c>
+      <c r="B100">
+        <v>580</v>
+      </c>
+      <c r="C100">
+        <v>2881</v>
+      </c>
+      <c r="D100">
+        <v>450</v>
+      </c>
+      <c r="E100">
+        <v>5177</v>
+      </c>
+      <c r="F100">
+        <v>20</v>
+      </c>
+      <c r="G100">
+        <v>2153</v>
+      </c>
+      <c r="H100">
+        <v>1000</v>
+      </c>
+      <c r="I100">
+        <v>28500</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <v>3674</v>
+      </c>
+      <c r="N100">
+        <v>84</v>
+      </c>
+      <c r="O100">
+        <v>1166</v>
+      </c>
+      <c r="P100">
+        <v>42385</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2">
+        <v>44343</v>
+      </c>
+      <c r="B101">
+        <v>785</v>
+      </c>
+      <c r="C101">
+        <v>2761</v>
+      </c>
+      <c r="D101">
+        <v>750</v>
+      </c>
+      <c r="E101">
+        <v>5027</v>
+      </c>
+      <c r="F101">
+        <v>441</v>
+      </c>
+      <c r="G101">
+        <v>2163</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+      <c r="I101">
+        <v>28500</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+      <c r="M101">
+        <v>3674</v>
+      </c>
+      <c r="N101">
+        <v>463</v>
+      </c>
+      <c r="O101">
+        <v>1153</v>
+      </c>
+      <c r="P101">
+        <v>42125</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2">
+        <v>44344</v>
+      </c>
+      <c r="B102">
+        <v>440</v>
+      </c>
+      <c r="C102">
+        <v>2851</v>
+      </c>
+      <c r="D102">
+        <v>1144</v>
+      </c>
+      <c r="E102">
+        <v>5121</v>
+      </c>
+      <c r="F102">
+        <v>525</v>
+      </c>
+      <c r="G102">
+        <v>2171</v>
+      </c>
+      <c r="H102">
+        <v>1000</v>
+      </c>
+      <c r="I102">
+        <v>28500</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102">
+        <v>3674</v>
+      </c>
+      <c r="N102">
+        <v>13</v>
+      </c>
+      <c r="O102">
+        <v>1142</v>
+      </c>
+      <c r="P102">
+        <v>42317</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2">
+        <v>44347</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+      <c r="C103">
+        <v>2851</v>
+      </c>
+      <c r="D103">
+        <v>286</v>
+      </c>
+      <c r="E103">
+        <v>5407</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>2171</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+      <c r="I103">
+        <v>28500</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103">
+        <v>3674</v>
+      </c>
+      <c r="N103">
+        <v>0</v>
+      </c>
+      <c r="O103">
+        <v>1142</v>
+      </c>
+      <c r="P103">
+        <v>42603</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2">
+        <v>44348</v>
+      </c>
+      <c r="B104">
+        <v>300</v>
+      </c>
+      <c r="C104">
+        <v>2736</v>
+      </c>
+      <c r="D104">
+        <v>900</v>
+      </c>
+      <c r="E104">
+        <v>5557</v>
+      </c>
+      <c r="F104">
+        <v>214</v>
+      </c>
+      <c r="G104">
+        <v>2167</v>
+      </c>
+      <c r="H104">
+        <v>1500</v>
+      </c>
+      <c r="I104">
+        <v>28500</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104">
+        <v>3674</v>
+      </c>
+      <c r="N104">
+        <v>123</v>
+      </c>
+      <c r="O104">
+        <v>1039</v>
+      </c>
+      <c r="P104">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2">
+        <v>44349</v>
+      </c>
+      <c r="B105">
+        <v>755</v>
+      </c>
+      <c r="C105">
+        <v>2911</v>
+      </c>
+      <c r="D105">
+        <v>1627</v>
+      </c>
+      <c r="E105">
+        <v>6157</v>
+      </c>
+      <c r="F105">
+        <v>50</v>
+      </c>
+      <c r="G105">
+        <v>2198</v>
+      </c>
+      <c r="H105">
+        <v>1000</v>
+      </c>
+      <c r="I105">
+        <v>28500</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
+        <v>3674</v>
+      </c>
+      <c r="N105">
+        <v>85</v>
+      </c>
+      <c r="O105">
+        <v>1040</v>
+      </c>
+      <c r="P105">
+        <v>43440</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2">
+        <v>44350</v>
+      </c>
+      <c r="B106">
+        <v>866</v>
+      </c>
+      <c r="C106">
+        <v>2992</v>
+      </c>
+      <c r="D106">
+        <v>1261</v>
+      </c>
+      <c r="E106">
+        <v>6518</v>
+      </c>
+      <c r="F106">
+        <v>439</v>
+      </c>
+      <c r="G106">
+        <v>2196</v>
+      </c>
+      <c r="H106">
+        <v>0</v>
+      </c>
+      <c r="I106">
+        <v>28500</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106">
+        <v>3674</v>
+      </c>
+      <c r="N106">
+        <v>509</v>
+      </c>
+      <c r="O106">
+        <v>1087</v>
+      </c>
+      <c r="P106">
+        <v>43880</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2021-06-10 14:03:31 - Update
</commit_message>
<xml_diff>
--- a/swap.xlsx
+++ b/swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P106"/>
+  <dimension ref="A1:P110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5696,6 +5696,206 @@
         <v>43880</v>
       </c>
     </row>
+    <row r="107">
+      <c r="A107" s="2">
+        <v>44351</v>
+      </c>
+      <c r="B107">
+        <v>600</v>
+      </c>
+      <c r="C107">
+        <v>3152</v>
+      </c>
+      <c r="D107">
+        <v>911</v>
+      </c>
+      <c r="E107">
+        <v>6879</v>
+      </c>
+      <c r="F107">
+        <v>524</v>
+      </c>
+      <c r="G107">
+        <v>2195</v>
+      </c>
+      <c r="H107">
+        <v>0</v>
+      </c>
+      <c r="I107">
+        <v>28500</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107">
+        <v>3674</v>
+      </c>
+      <c r="N107">
+        <v>13</v>
+      </c>
+      <c r="O107">
+        <v>1087</v>
+      </c>
+      <c r="P107">
+        <v>44400</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2">
+        <v>44354</v>
+      </c>
+      <c r="B108">
+        <v>902</v>
+      </c>
+      <c r="C108">
+        <v>3423</v>
+      </c>
+      <c r="D108">
+        <v>572</v>
+      </c>
+      <c r="E108">
+        <v>6258</v>
+      </c>
+      <c r="F108">
+        <v>1066</v>
+      </c>
+      <c r="G108">
+        <v>2293</v>
+      </c>
+      <c r="H108">
+        <v>1000</v>
+      </c>
+      <c r="I108">
+        <v>28500</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108">
+        <v>3674</v>
+      </c>
+      <c r="N108">
+        <v>278</v>
+      </c>
+      <c r="O108">
+        <v>1008</v>
+      </c>
+      <c r="P108">
+        <v>44148</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2">
+        <v>44355</v>
+      </c>
+      <c r="B109">
+        <v>400</v>
+      </c>
+      <c r="C109">
+        <v>3523</v>
+      </c>
+      <c r="D109">
+        <v>854</v>
+      </c>
+      <c r="E109">
+        <v>6275</v>
+      </c>
+      <c r="F109">
+        <v>212</v>
+      </c>
+      <c r="G109">
+        <v>2291</v>
+      </c>
+      <c r="H109">
+        <v>0</v>
+      </c>
+      <c r="I109">
+        <v>28500</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>0</v>
+      </c>
+      <c r="M109">
+        <v>3674</v>
+      </c>
+      <c r="N109">
+        <v>122</v>
+      </c>
+      <c r="O109">
+        <v>1008</v>
+      </c>
+      <c r="P109">
+        <v>44263</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2">
+        <v>44356</v>
+      </c>
+      <c r="B110">
+        <v>930</v>
+      </c>
+      <c r="C110">
+        <v>3698</v>
+      </c>
+      <c r="D110">
+        <v>700</v>
+      </c>
+      <c r="E110">
+        <v>6275</v>
+      </c>
+      <c r="F110">
+        <v>75</v>
+      </c>
+      <c r="G110">
+        <v>2316</v>
+      </c>
+      <c r="H110">
+        <v>0</v>
+      </c>
+      <c r="I110">
+        <v>28500</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+      <c r="K110">
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <v>0</v>
+      </c>
+      <c r="M110">
+        <v>3674</v>
+      </c>
+      <c r="N110">
+        <v>77</v>
+      </c>
+      <c r="O110">
+        <v>999</v>
+      </c>
+      <c r="P110">
+        <v>44463</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2021-06-13 18:51:54 - Update
</commit_message>
<xml_diff>
--- a/swap.xlsx
+++ b/swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P110"/>
+  <dimension ref="A1:P112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5896,6 +5896,106 @@
         <v>44463</v>
       </c>
     </row>
+    <row r="111">
+      <c r="A111" s="2">
+        <v>44357</v>
+      </c>
+      <c r="B111">
+        <v>976</v>
+      </c>
+      <c r="C111">
+        <v>3808</v>
+      </c>
+      <c r="D111">
+        <v>1182</v>
+      </c>
+      <c r="E111">
+        <v>6585</v>
+      </c>
+      <c r="F111">
+        <v>438</v>
+      </c>
+      <c r="G111">
+        <v>2315</v>
+      </c>
+      <c r="H111">
+        <v>1000</v>
+      </c>
+      <c r="I111">
+        <v>28500</v>
+      </c>
+      <c r="J111">
+        <v>0</v>
+      </c>
+      <c r="K111">
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <v>0</v>
+      </c>
+      <c r="M111">
+        <v>3674</v>
+      </c>
+      <c r="N111">
+        <v>420</v>
+      </c>
+      <c r="O111">
+        <v>910</v>
+      </c>
+      <c r="P111">
+        <v>44881</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2">
+        <v>44358</v>
+      </c>
+      <c r="B112">
+        <v>1050</v>
+      </c>
+      <c r="C112">
+        <v>4258</v>
+      </c>
+      <c r="D112">
+        <v>905</v>
+      </c>
+      <c r="E112">
+        <v>6485</v>
+      </c>
+      <c r="F112">
+        <v>496</v>
+      </c>
+      <c r="G112">
+        <v>2287</v>
+      </c>
+      <c r="H112">
+        <v>0</v>
+      </c>
+      <c r="I112">
+        <v>28500</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
+      </c>
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+      <c r="M112">
+        <v>3674</v>
+      </c>
+      <c r="N112">
+        <v>61</v>
+      </c>
+      <c r="O112">
+        <v>959</v>
+      </c>
+      <c r="P112">
+        <v>45204</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
2021-07-28 13:28:19 - Update
</commit_message>
<xml_diff>
--- a/swap.xlsx
+++ b/swap.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P112"/>
+  <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5996,6 +5996,1356 @@
         <v>45204</v>
       </c>
     </row>
+    <row r="113">
+      <c r="A113" s="2">
+        <v>44361</v>
+      </c>
+      <c r="B113">
+        <v>502</v>
+      </c>
+      <c r="C113">
+        <v>3858</v>
+      </c>
+      <c r="D113">
+        <v>397</v>
+      </c>
+      <c r="E113">
+        <v>6082</v>
+      </c>
+      <c r="F113">
+        <v>862</v>
+      </c>
+      <c r="G113">
+        <v>2083</v>
+      </c>
+      <c r="H113">
+        <v>1000</v>
+      </c>
+      <c r="I113">
+        <v>28500</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
+      </c>
+      <c r="K113">
+        <v>0</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113">
+        <v>3674</v>
+      </c>
+      <c r="N113">
+        <v>179</v>
+      </c>
+      <c r="O113">
+        <v>860</v>
+      </c>
+      <c r="P113">
+        <v>44197</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2">
+        <v>44362</v>
+      </c>
+      <c r="B114">
+        <v>500</v>
+      </c>
+      <c r="C114">
+        <v>3958</v>
+      </c>
+      <c r="D114">
+        <v>1404</v>
+      </c>
+      <c r="E114">
+        <v>6092</v>
+      </c>
+      <c r="F114">
+        <v>254</v>
+      </c>
+      <c r="G114">
+        <v>2125</v>
+      </c>
+      <c r="H114">
+        <v>1000</v>
+      </c>
+      <c r="I114">
+        <v>28500</v>
+      </c>
+      <c r="J114">
+        <v>0</v>
+      </c>
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>1232</v>
+      </c>
+      <c r="M114">
+        <v>3787</v>
+      </c>
+      <c r="N114">
+        <v>121</v>
+      </c>
+      <c r="O114">
+        <v>858</v>
+      </c>
+      <c r="P114">
+        <v>44462</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2">
+        <v>44363</v>
+      </c>
+      <c r="B115">
+        <v>780</v>
+      </c>
+      <c r="C115">
+        <v>3808</v>
+      </c>
+      <c r="D115">
+        <v>1714</v>
+      </c>
+      <c r="E115">
+        <v>6752</v>
+      </c>
+      <c r="F115">
+        <v>74</v>
+      </c>
+      <c r="G115">
+        <v>2124</v>
+      </c>
+      <c r="H115">
+        <v>1000</v>
+      </c>
+      <c r="I115">
+        <v>28500</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115">
+        <v>3787</v>
+      </c>
+      <c r="N115">
+        <v>76</v>
+      </c>
+      <c r="O115">
+        <v>857</v>
+      </c>
+      <c r="P115">
+        <v>44971</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2">
+        <v>44364</v>
+      </c>
+      <c r="B116">
+        <v>1051</v>
+      </c>
+      <c r="C116">
+        <v>3883</v>
+      </c>
+      <c r="D116">
+        <v>1141</v>
+      </c>
+      <c r="E116">
+        <v>7093</v>
+      </c>
+      <c r="F116">
+        <v>413</v>
+      </c>
+      <c r="G116">
+        <v>2099</v>
+      </c>
+      <c r="H116">
+        <v>0</v>
+      </c>
+      <c r="I116">
+        <v>28500</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
+      </c>
+      <c r="K116">
+        <v>0</v>
+      </c>
+      <c r="L116">
+        <v>0</v>
+      </c>
+      <c r="M116">
+        <v>3787</v>
+      </c>
+      <c r="N116">
+        <v>443</v>
+      </c>
+      <c r="O116">
+        <v>880</v>
+      </c>
+      <c r="P116">
+        <v>45361</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2">
+        <v>44365</v>
+      </c>
+      <c r="B117">
+        <v>721</v>
+      </c>
+      <c r="C117">
+        <v>3554</v>
+      </c>
+      <c r="D117">
+        <v>1895</v>
+      </c>
+      <c r="E117">
+        <v>7756</v>
+      </c>
+      <c r="F117">
+        <v>535</v>
+      </c>
+      <c r="G117">
+        <v>2138</v>
+      </c>
+      <c r="H117">
+        <v>1500</v>
+      </c>
+      <c r="I117">
+        <v>28500</v>
+      </c>
+      <c r="J117">
+        <v>0</v>
+      </c>
+      <c r="K117">
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <v>0</v>
+      </c>
+      <c r="M117">
+        <v>3787</v>
+      </c>
+      <c r="N117">
+        <v>0</v>
+      </c>
+      <c r="O117">
+        <v>819</v>
+      </c>
+      <c r="P117">
+        <v>45735</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2">
+        <v>44368</v>
+      </c>
+      <c r="B118">
+        <v>527</v>
+      </c>
+      <c r="C118">
+        <v>3579</v>
+      </c>
+      <c r="D118">
+        <v>774</v>
+      </c>
+      <c r="E118">
+        <v>7625</v>
+      </c>
+      <c r="F118">
+        <v>768</v>
+      </c>
+      <c r="G118">
+        <v>2044</v>
+      </c>
+      <c r="H118">
+        <v>1000</v>
+      </c>
+      <c r="I118">
+        <v>28500</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+      <c r="K118">
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118">
+        <v>3787</v>
+      </c>
+      <c r="N118">
+        <v>170</v>
+      </c>
+      <c r="O118">
+        <v>809</v>
+      </c>
+      <c r="P118">
+        <v>45535</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2">
+        <v>44369</v>
+      </c>
+      <c r="B119">
+        <v>200</v>
+      </c>
+      <c r="C119">
+        <v>3279</v>
+      </c>
+      <c r="D119">
+        <v>399</v>
+      </c>
+      <c r="E119">
+        <v>7574</v>
+      </c>
+      <c r="F119">
+        <v>204</v>
+      </c>
+      <c r="G119">
+        <v>1994</v>
+      </c>
+      <c r="H119">
+        <v>1500</v>
+      </c>
+      <c r="I119">
+        <v>28500</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
+      </c>
+      <c r="M119">
+        <v>3787</v>
+      </c>
+      <c r="N119">
+        <v>133</v>
+      </c>
+      <c r="O119">
+        <v>821</v>
+      </c>
+      <c r="P119">
+        <v>45134</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2">
+        <v>44370</v>
+      </c>
+      <c r="B120">
+        <v>705</v>
+      </c>
+      <c r="C120">
+        <v>3204</v>
+      </c>
+      <c r="D120">
+        <v>1325</v>
+      </c>
+      <c r="E120">
+        <v>7773</v>
+      </c>
+      <c r="F120">
+        <v>31</v>
+      </c>
+      <c r="G120">
+        <v>1951</v>
+      </c>
+      <c r="H120">
+        <v>1000</v>
+      </c>
+      <c r="I120">
+        <v>28500</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>0</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
+      </c>
+      <c r="M120">
+        <v>3787</v>
+      </c>
+      <c r="N120">
+        <v>115</v>
+      </c>
+      <c r="O120">
+        <v>861</v>
+      </c>
+      <c r="P120">
+        <v>45215</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2">
+        <v>44371</v>
+      </c>
+      <c r="B121">
+        <v>900</v>
+      </c>
+      <c r="C121">
+        <v>3053</v>
+      </c>
+      <c r="D121">
+        <v>1598</v>
+      </c>
+      <c r="E121">
+        <v>8132</v>
+      </c>
+      <c r="F121">
+        <v>299</v>
+      </c>
+      <c r="G121">
+        <v>1838</v>
+      </c>
+      <c r="H121">
+        <v>0</v>
+      </c>
+      <c r="I121">
+        <v>28500</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="K121">
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="M121">
+        <v>3787</v>
+      </c>
+      <c r="N121">
+        <v>353</v>
+      </c>
+      <c r="O121">
+        <v>771</v>
+      </c>
+      <c r="P121">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2">
+        <v>44372</v>
+      </c>
+      <c r="B122">
+        <v>725</v>
+      </c>
+      <c r="C122">
+        <v>3057</v>
+      </c>
+      <c r="D122">
+        <v>1010</v>
+      </c>
+      <c r="E122">
+        <v>8331</v>
+      </c>
+      <c r="F122">
+        <v>527</v>
+      </c>
+      <c r="G122">
+        <v>1829</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>28500</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <v>0</v>
+      </c>
+      <c r="M122">
+        <v>3787</v>
+      </c>
+      <c r="N122">
+        <v>0</v>
+      </c>
+      <c r="O122">
+        <v>771</v>
+      </c>
+      <c r="P122">
+        <v>45503</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2">
+        <v>44375</v>
+      </c>
+      <c r="B123">
+        <v>495</v>
+      </c>
+      <c r="C123">
+        <v>3025</v>
+      </c>
+      <c r="D123">
+        <v>553</v>
+      </c>
+      <c r="E123">
+        <v>8028</v>
+      </c>
+      <c r="F123">
+        <v>751</v>
+      </c>
+      <c r="G123">
+        <v>1812</v>
+      </c>
+      <c r="H123">
+        <v>1500</v>
+      </c>
+      <c r="I123">
+        <v>28500</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+      <c r="K123">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123">
+        <v>3787</v>
+      </c>
+      <c r="N123">
+        <v>204</v>
+      </c>
+      <c r="O123">
+        <v>805</v>
+      </c>
+      <c r="P123">
+        <v>45152</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2">
+        <v>44376</v>
+      </c>
+      <c r="B124">
+        <v>550</v>
+      </c>
+      <c r="C124">
+        <v>3375</v>
+      </c>
+      <c r="D124">
+        <v>479</v>
+      </c>
+      <c r="E124">
+        <v>7338</v>
+      </c>
+      <c r="F124">
+        <v>203</v>
+      </c>
+      <c r="G124">
+        <v>1811</v>
+      </c>
+      <c r="H124">
+        <v>1000</v>
+      </c>
+      <c r="I124">
+        <v>28500</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124">
+        <v>3787</v>
+      </c>
+      <c r="N124">
+        <v>132</v>
+      </c>
+      <c r="O124">
+        <v>805</v>
+      </c>
+      <c r="P124">
+        <v>44811</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2">
+        <v>44377</v>
+      </c>
+      <c r="B125">
+        <v>600</v>
+      </c>
+      <c r="C125">
+        <v>3270</v>
+      </c>
+      <c r="D125">
+        <v>1124</v>
+      </c>
+      <c r="E125">
+        <v>7338</v>
+      </c>
+      <c r="F125">
+        <v>15</v>
+      </c>
+      <c r="G125">
+        <v>1794</v>
+      </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125">
+        <v>28500</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
+      </c>
+      <c r="K125">
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+      <c r="M125">
+        <v>3787</v>
+      </c>
+      <c r="N125">
+        <v>115</v>
+      </c>
+      <c r="O125">
+        <v>804</v>
+      </c>
+      <c r="P125">
+        <v>44689</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2">
+        <v>44378</v>
+      </c>
+      <c r="B126">
+        <v>700</v>
+      </c>
+      <c r="C126">
+        <v>3070</v>
+      </c>
+      <c r="D126">
+        <v>1122</v>
+      </c>
+      <c r="E126">
+        <v>7398</v>
+      </c>
+      <c r="F126">
+        <v>281</v>
+      </c>
+      <c r="G126">
+        <v>1776</v>
+      </c>
+      <c r="H126">
+        <v>1000</v>
+      </c>
+      <c r="I126">
+        <v>28500</v>
+      </c>
+      <c r="J126">
+        <v>0</v>
+      </c>
+      <c r="K126">
+        <v>0</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
+      </c>
+      <c r="M126">
+        <v>3787</v>
+      </c>
+      <c r="N126">
+        <v>281</v>
+      </c>
+      <c r="O126">
+        <v>732</v>
+      </c>
+      <c r="P126">
+        <v>44531</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2">
+        <v>44379</v>
+      </c>
+      <c r="B127">
+        <v>640</v>
+      </c>
+      <c r="C127">
+        <v>2985</v>
+      </c>
+      <c r="D127">
+        <v>1156</v>
+      </c>
+      <c r="E127">
+        <v>7721</v>
+      </c>
+      <c r="F127">
+        <v>524</v>
+      </c>
+      <c r="G127">
+        <v>1774</v>
+      </c>
+      <c r="H127">
+        <v>1000</v>
+      </c>
+      <c r="I127">
+        <v>28500</v>
+      </c>
+      <c r="J127">
+        <v>0</v>
+      </c>
+      <c r="K127">
+        <v>0</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+      <c r="M127">
+        <v>3787</v>
+      </c>
+      <c r="N127">
+        <v>77</v>
+      </c>
+      <c r="O127">
+        <v>809</v>
+      </c>
+      <c r="P127">
+        <v>44766</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2">
+        <v>44382</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+      <c r="C128">
+        <v>2985</v>
+      </c>
+      <c r="D128">
+        <v>237</v>
+      </c>
+      <c r="E128">
+        <v>7719</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+      <c r="G128">
+        <v>1774</v>
+      </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>28500</v>
+      </c>
+      <c r="J128">
+        <v>0</v>
+      </c>
+      <c r="K128">
+        <v>0</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+      <c r="M128">
+        <v>3787</v>
+      </c>
+      <c r="N128">
+        <v>0</v>
+      </c>
+      <c r="O128">
+        <v>809</v>
+      </c>
+      <c r="P128">
+        <v>44764</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2">
+        <v>44383</v>
+      </c>
+      <c r="B129">
+        <v>800</v>
+      </c>
+      <c r="C129">
+        <v>3235</v>
+      </c>
+      <c r="D129">
+        <v>1275</v>
+      </c>
+      <c r="E129">
+        <v>7476</v>
+      </c>
+      <c r="F129">
+        <v>205</v>
+      </c>
+      <c r="G129">
+        <v>1775</v>
+      </c>
+      <c r="H129">
+        <v>1000</v>
+      </c>
+      <c r="I129">
+        <v>28500</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+      <c r="K129">
+        <v>0</v>
+      </c>
+      <c r="L129">
+        <v>0</v>
+      </c>
+      <c r="M129">
+        <v>3787</v>
+      </c>
+      <c r="N129">
+        <v>134</v>
+      </c>
+      <c r="O129">
+        <v>810</v>
+      </c>
+      <c r="P129">
+        <v>44773</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2">
+        <v>44384</v>
+      </c>
+      <c r="B130">
+        <v>680</v>
+      </c>
+      <c r="C130">
+        <v>3315</v>
+      </c>
+      <c r="D130">
+        <v>1376</v>
+      </c>
+      <c r="E130">
+        <v>7749</v>
+      </c>
+      <c r="F130">
+        <v>14</v>
+      </c>
+      <c r="G130">
+        <v>1775</v>
+      </c>
+      <c r="H130">
+        <v>1000</v>
+      </c>
+      <c r="I130">
+        <v>28500</v>
+      </c>
+      <c r="J130">
+        <v>0</v>
+      </c>
+      <c r="K130">
+        <v>0</v>
+      </c>
+      <c r="L130">
+        <v>0</v>
+      </c>
+      <c r="M130">
+        <v>3787</v>
+      </c>
+      <c r="N130">
+        <v>45</v>
+      </c>
+      <c r="O130">
+        <v>740</v>
+      </c>
+      <c r="P130">
+        <v>45125</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2">
+        <v>44385</v>
+      </c>
+      <c r="B131">
+        <v>1010</v>
+      </c>
+      <c r="C131">
+        <v>3625</v>
+      </c>
+      <c r="D131">
+        <v>1087</v>
+      </c>
+      <c r="E131">
+        <v>7177</v>
+      </c>
+      <c r="F131">
+        <v>288</v>
+      </c>
+      <c r="G131">
+        <v>1782</v>
+      </c>
+      <c r="H131">
+        <v>0</v>
+      </c>
+      <c r="I131">
+        <v>28500</v>
+      </c>
+      <c r="J131">
+        <v>0</v>
+      </c>
+      <c r="K131">
+        <v>0</v>
+      </c>
+      <c r="L131">
+        <v>0</v>
+      </c>
+      <c r="M131">
+        <v>3787</v>
+      </c>
+      <c r="N131">
+        <v>248</v>
+      </c>
+      <c r="O131">
+        <v>707</v>
+      </c>
+      <c r="P131">
+        <v>44871</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2">
+        <v>44386</v>
+      </c>
+      <c r="B132">
+        <v>520</v>
+      </c>
+      <c r="C132">
+        <v>3505</v>
+      </c>
+      <c r="D132">
+        <v>587</v>
+      </c>
+      <c r="E132">
+        <v>6995</v>
+      </c>
+      <c r="F132">
+        <v>463</v>
+      </c>
+      <c r="G132">
+        <v>1721</v>
+      </c>
+      <c r="H132">
+        <v>0</v>
+      </c>
+      <c r="I132">
+        <v>28500</v>
+      </c>
+      <c r="J132">
+        <v>0</v>
+      </c>
+      <c r="K132">
+        <v>0</v>
+      </c>
+      <c r="L132">
+        <v>0</v>
+      </c>
+      <c r="M132">
+        <v>3787</v>
+      </c>
+      <c r="N132">
+        <v>0</v>
+      </c>
+      <c r="O132">
+        <v>630</v>
+      </c>
+      <c r="P132">
+        <v>44508</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2">
+        <v>44389</v>
+      </c>
+      <c r="B133">
+        <v>237</v>
+      </c>
+      <c r="C133">
+        <v>3247</v>
+      </c>
+      <c r="D133">
+        <v>1029</v>
+      </c>
+      <c r="E133">
+        <v>6941</v>
+      </c>
+      <c r="F133">
+        <v>754</v>
+      </c>
+      <c r="G133">
+        <v>1724</v>
+      </c>
+      <c r="H133">
+        <v>1000</v>
+      </c>
+      <c r="I133">
+        <v>28500</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
+      <c r="L133">
+        <v>0</v>
+      </c>
+      <c r="M133">
+        <v>3787</v>
+      </c>
+      <c r="N133">
+        <v>148</v>
+      </c>
+      <c r="O133">
+        <v>574</v>
+      </c>
+      <c r="P133">
+        <v>44199</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2">
+        <v>44390</v>
+      </c>
+      <c r="B134">
+        <v>975</v>
+      </c>
+      <c r="C134">
+        <v>3422</v>
+      </c>
+      <c r="D134">
+        <v>831</v>
+      </c>
+      <c r="E134">
+        <v>7050</v>
+      </c>
+      <c r="F134">
+        <v>206</v>
+      </c>
+      <c r="G134">
+        <v>1726</v>
+      </c>
+      <c r="H134">
+        <v>1000</v>
+      </c>
+      <c r="I134">
+        <v>28500</v>
+      </c>
+      <c r="J134">
+        <v>0</v>
+      </c>
+      <c r="K134">
+        <v>0</v>
+      </c>
+      <c r="L134">
+        <v>0</v>
+      </c>
+      <c r="M134">
+        <v>3787</v>
+      </c>
+      <c r="N134">
+        <v>74</v>
+      </c>
+      <c r="O134">
+        <v>515</v>
+      </c>
+      <c r="P134">
+        <v>44485</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2">
+        <v>44391</v>
+      </c>
+      <c r="B135">
+        <v>850</v>
+      </c>
+      <c r="C135">
+        <v>3592</v>
+      </c>
+      <c r="D135">
+        <v>987</v>
+      </c>
+      <c r="E135">
+        <v>6721</v>
+      </c>
+      <c r="F135">
+        <v>14</v>
+      </c>
+      <c r="G135">
+        <v>1726</v>
+      </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
+      <c r="I135">
+        <v>28500</v>
+      </c>
+      <c r="J135">
+        <v>0</v>
+      </c>
+      <c r="K135">
+        <v>0</v>
+      </c>
+      <c r="L135">
+        <v>0</v>
+      </c>
+      <c r="M135">
+        <v>3787</v>
+      </c>
+      <c r="N135">
+        <v>43</v>
+      </c>
+      <c r="O135">
+        <v>514</v>
+      </c>
+      <c r="P135">
+        <v>44325</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2">
+        <v>44393</v>
+      </c>
+      <c r="B136">
+        <v>1685</v>
+      </c>
+      <c r="C136">
+        <v>3747</v>
+      </c>
+      <c r="D136">
+        <v>1404</v>
+      </c>
+      <c r="E136">
+        <v>7000</v>
+      </c>
+      <c r="F136">
+        <v>763</v>
+      </c>
+      <c r="G136">
+        <v>1738</v>
+      </c>
+      <c r="H136">
+        <v>1000</v>
+      </c>
+      <c r="I136">
+        <v>28500</v>
+      </c>
+      <c r="J136">
+        <v>0</v>
+      </c>
+      <c r="K136">
+        <v>0</v>
+      </c>
+      <c r="L136">
+        <v>0</v>
+      </c>
+      <c r="M136">
+        <v>3787</v>
+      </c>
+      <c r="N136">
+        <v>252</v>
+      </c>
+      <c r="O136">
+        <v>517</v>
+      </c>
+      <c r="P136">
+        <v>44771</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2">
+        <v>44396</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+      <c r="C137">
+        <v>3747</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>7000</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="G137">
+        <v>1738</v>
+      </c>
+      <c r="H137">
+        <v>0</v>
+      </c>
+      <c r="I137">
+        <v>28500</v>
+      </c>
+      <c r="J137">
+        <v>0</v>
+      </c>
+      <c r="K137">
+        <v>0</v>
+      </c>
+      <c r="L137">
+        <v>0</v>
+      </c>
+      <c r="M137">
+        <v>3787</v>
+      </c>
+      <c r="N137">
+        <v>0</v>
+      </c>
+      <c r="O137">
+        <v>517</v>
+      </c>
+      <c r="P137">
+        <v>44771</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2">
+        <v>44403</v>
+      </c>
+      <c r="B138">
+        <v>612</v>
+      </c>
+      <c r="C138">
+        <v>4122</v>
+      </c>
+      <c r="D138">
+        <v>1096</v>
+      </c>
+      <c r="E138">
+        <v>6688</v>
+      </c>
+      <c r="F138">
+        <v>768</v>
+      </c>
+      <c r="G138">
+        <v>1752</v>
+      </c>
+      <c r="H138">
+        <v>1000</v>
+      </c>
+      <c r="I138">
+        <v>28500</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+      <c r="K138">
+        <v>0</v>
+      </c>
+      <c r="L138">
+        <v>0</v>
+      </c>
+      <c r="M138">
+        <v>3787</v>
+      </c>
+      <c r="N138">
+        <v>148</v>
+      </c>
+      <c r="O138">
+        <v>517</v>
+      </c>
+      <c r="P138">
+        <v>44849</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2">
+        <v>44404</v>
+      </c>
+      <c r="B139">
+        <v>1020</v>
+      </c>
+      <c r="C139">
+        <v>4167</v>
+      </c>
+      <c r="D139">
+        <v>997</v>
+      </c>
+      <c r="E139">
+        <v>6957</v>
+      </c>
+      <c r="F139">
+        <v>200</v>
+      </c>
+      <c r="G139">
+        <v>1745</v>
+      </c>
+      <c r="H139">
+        <v>1000</v>
+      </c>
+      <c r="I139">
+        <v>28500</v>
+      </c>
+      <c r="J139">
+        <v>0</v>
+      </c>
+      <c r="K139">
+        <v>0</v>
+      </c>
+      <c r="L139">
+        <v>0</v>
+      </c>
+      <c r="M139">
+        <v>3787</v>
+      </c>
+      <c r="N139">
+        <v>76</v>
+      </c>
+      <c r="O139">
+        <v>520</v>
+      </c>
+      <c r="P139">
+        <v>45156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>